<commit_message>
fixed error for other file
</commit_message>
<xml_diff>
--- a/static/finalOutput/alert.xlsx
+++ b/static/finalOutput/alert.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>PART NO.</t>
   </si>
@@ -25,106 +25,157 @@
     <t>alert</t>
   </si>
   <si>
-    <t>CPA110Y-NFS5G-9NNNN/T12</t>
-  </si>
-  <si>
-    <t>CPA110Y-NFS5G-BNNNN/T12</t>
-  </si>
-  <si>
-    <t>CPA110Y-NFS5J-BNNNN</t>
-  </si>
-  <si>
-    <t>CPA110Y-NHA5G-9NNNN</t>
-  </si>
-  <si>
-    <t>CPA110Y-NHH5G-9NNNN</t>
-  </si>
-  <si>
-    <t>CPA110Y-NHH5J-9NNNN</t>
-  </si>
-  <si>
-    <t>CPA110Y-NMA5G-9NNNN/K3</t>
-  </si>
-  <si>
-    <t>CPA110Y-NMA5G-9NNNN/T12</t>
-  </si>
-  <si>
-    <t>CPA110Y-NMT5G-8NNNN</t>
-  </si>
-  <si>
-    <t>CPA430Y-NAB5J-9NNNN/T01</t>
-  </si>
-  <si>
-    <t>CPA530Y-NAH4N-0NNNN/T05</t>
-  </si>
-  <si>
-    <t>CPA530Y-NAS4N-0NNNN/T05</t>
-  </si>
-  <si>
-    <t>CPA530Y-NBS4N-0NNNN/K1</t>
-  </si>
-  <si>
-    <t>CPA530Y-NBS4N-0NNNN/T06</t>
-  </si>
-  <si>
-    <t>CPA530Y-NBS7N-0NNNN/T06</t>
-  </si>
-  <si>
-    <t>CPA530Y-NCS4N-0NNNN/T07</t>
-  </si>
-  <si>
-    <t>CPA530Y-NCS4N-0NNNN/T07/A1</t>
-  </si>
-  <si>
-    <t>CPA530Y-NCS7N-0NNNN</t>
-  </si>
-  <si>
-    <t>CPA530Y-NDS4N-0NNNN/T08</t>
-  </si>
-  <si>
-    <t>CPA530Y-NDS4N-0NNNN/T08/A1</t>
-  </si>
-  <si>
-    <t>CPA530Y-NDS8N-0NNNN</t>
-  </si>
-  <si>
-    <t>F9340SC</t>
+    <t>CPA110Y-NMSNN-NNNNN</t>
+  </si>
+  <si>
+    <t>D0114RB</t>
+  </si>
+  <si>
+    <t>D0117XL-A</t>
+  </si>
+  <si>
+    <t>F9270BJ</t>
+  </si>
+  <si>
+    <t>F9270BK</t>
+  </si>
+  <si>
+    <t>F9273CZ</t>
+  </si>
+  <si>
+    <t>F9300AF</t>
+  </si>
+  <si>
+    <t>F9300TE</t>
+  </si>
+  <si>
+    <t>F9340XX</t>
+  </si>
+  <si>
+    <t>F9341JA</t>
+  </si>
+  <si>
+    <t>F9341JD</t>
+  </si>
+  <si>
+    <t>F9341JE</t>
+  </si>
+  <si>
+    <t>F9341JP</t>
+  </si>
+  <si>
+    <t>F9341JQ</t>
+  </si>
+  <si>
+    <t>F9341JS</t>
+  </si>
+  <si>
+    <t>F9341JW</t>
+  </si>
+  <si>
+    <t>F9341JZ</t>
   </si>
   <si>
     <t>F9342MK</t>
   </si>
   <si>
-    <t>F9900GK</t>
-  </si>
-  <si>
-    <t>F9900TC</t>
-  </si>
-  <si>
-    <t>F9900TE</t>
-  </si>
-  <si>
-    <t>F9903BH</t>
-  </si>
-  <si>
-    <t>F9903CP</t>
-  </si>
-  <si>
-    <t>F9903DB</t>
-  </si>
-  <si>
-    <t>F9913AJ</t>
-  </si>
-  <si>
-    <t>F9913QA</t>
+    <t>F9342NJ</t>
+  </si>
+  <si>
+    <t>F9342YB</t>
+  </si>
+  <si>
+    <t>F9900AC</t>
+  </si>
+  <si>
+    <t>F9900AU</t>
+  </si>
+  <si>
+    <t>F9900BC</t>
+  </si>
+  <si>
+    <t>F9900EA</t>
+  </si>
+  <si>
+    <t>F9900GC</t>
+  </si>
+  <si>
+    <t>F9900GE</t>
+  </si>
+  <si>
+    <t>F9900GH</t>
+  </si>
+  <si>
+    <t>F9900GZ</t>
+  </si>
+  <si>
+    <t>F9900RE</t>
+  </si>
+  <si>
+    <t>F9900RF</t>
+  </si>
+  <si>
+    <t>F9900RG</t>
+  </si>
+  <si>
+    <t>F9900RJ</t>
+  </si>
+  <si>
+    <t>F9900RS</t>
+  </si>
+  <si>
+    <t>F9900TB</t>
+  </si>
+  <si>
+    <t>F9903BD</t>
+  </si>
+  <si>
+    <t>F9903CM</t>
+  </si>
+  <si>
+    <t>F9903CZ</t>
+  </si>
+  <si>
+    <t>F9910LE</t>
+  </si>
+  <si>
+    <t>F9910LS</t>
   </si>
   <si>
     <t>F9913QG</t>
   </si>
   <si>
-    <t>F9920TS</t>
-  </si>
-  <si>
-    <t>F9920VS</t>
+    <t>F9913QH</t>
+  </si>
+  <si>
+    <t>F9913TA</t>
+  </si>
+  <si>
+    <t>F9913TS</t>
+  </si>
+  <si>
+    <t>F9920LU</t>
+  </si>
+  <si>
+    <t>F9921AH</t>
+  </si>
+  <si>
+    <t>F9921VG</t>
+  </si>
+  <si>
+    <t>G9303NC</t>
+  </si>
+  <si>
+    <t>G9330DB</t>
+  </si>
+  <si>
+    <t>Y9308JY</t>
+  </si>
+  <si>
+    <t>Y9501WL</t>
+  </si>
+  <si>
+    <t>Y9812PS</t>
   </si>
   <si>
     <t>RED</t>
@@ -558,7 +609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,7 +631,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -589,473 +640,711 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>668</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>950</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1968</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2002</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3798</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>3027</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>927</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>656</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2031</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2031</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>2031</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1996</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2028</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2002</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1096</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1089</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>3975</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>475</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2276</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
       </c>
       <c r="C24">
-        <v>2616</v>
+        <v>2276</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>136</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>2096</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>160</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>3936</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
       </c>
       <c r="C27">
-        <v>46</v>
+        <v>1838</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>169</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1996</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>172</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>6795</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>175</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>2009</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1128</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>188</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>10093</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>189</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="C33">
-        <v>543</v>
+        <v>2002</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>211</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
       </c>
       <c r="C34">
-        <v>840</v>
+        <v>2009</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>217</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
       </c>
       <c r="C35">
-        <v>114</v>
+        <v>1522</v>
       </c>
       <c r="D35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>38</v>
       </c>
+      <c r="C37">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>83</v>
+      </c>
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>1996</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <v>2002</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41">
+        <v>777</v>
+      </c>
+      <c r="D41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42">
+        <v>983</v>
+      </c>
+      <c r="D42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43">
+        <v>1805</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44">
+        <v>1851</v>
+      </c>
+      <c r="D44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45">
+        <v>240</v>
+      </c>
+      <c r="D45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>159</v>
+      </c>
+      <c r="D46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47">
+        <v>25</v>
+      </c>
+      <c r="D47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48">
+        <v>1996</v>
+      </c>
+      <c r="D48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <v>4700</v>
+      </c>
+      <c r="D49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>4004</v>
+      </c>
+      <c r="D50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51">
+        <v>6006</v>
+      </c>
+      <c r="D51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52">
+        <v>2002</v>
+      </c>
+      <c r="D52" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D35">
+  <conditionalFormatting sqref="A1:D52">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>INDIRECT("D"&amp;ROW())="BLUE"</formula>
     </cfRule>

</xml_diff>